<commit_message>
Reset commit history due to disclosure
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Family ID</t>
   </si>
@@ -49,15 +49,6 @@
   </si>
   <si>
     <t>c</t>
-  </si>
-  <si>
-    <t>samojt@gmail.com</t>
-  </si>
-  <si>
-    <t>ydxcznbj@sharklasers.com</t>
-  </si>
-  <si>
-    <t>tomkinss@uni.coventry.ac.uk</t>
   </si>
   <si>
     <t>b1</t>
@@ -405,7 +396,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D5" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,9 +440,6 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
       <c r="E2">
         <v>0</v>
       </c>
@@ -473,9 +461,6 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3">
@@ -496,7 +481,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -520,9 +505,6 @@
       </c>
       <c r="C5" t="s">
         <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
       </c>
       <c r="E5">
         <v>2</v>

</xml_diff>